<commit_message>
Forgot about commits for a while
I did some test and adapted old ones
</commit_message>
<xml_diff>
--- a/sdi-entrega1-1105.xlsx
+++ b/sdi-entrega1-1105.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dio Brando\Documents\GitHub\sdi-entrega1-1105\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA07098-203D-40E4-AC5B-693D00E83F5B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98F1A5A-5651-4348-BDB4-25AF7C053C75}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -898,7 +898,7 @@
   <dimension ref="A1:I96"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -934,7 +934,7 @@
     <row r="4" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="40">
         <f>G31</f>
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="B4" s="40"/>
       <c r="C4" s="40"/>
@@ -980,7 +980,7 @@
     <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="23">
         <f>A4-A6</f>
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -1066,7 +1066,7 @@
       </c>
       <c r="D14" s="1">
         <f t="shared" ref="D14:D30" si="1">COUNTIFS($B$49:$B$96,$A14,$D$49:$D$96,"=OK")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" ref="E14:E30" si="2">COUNTIFS($B$49:$B$96,$A14,$D$49:$D$96,"FAIL")</f>
@@ -1074,11 +1074,11 @@
       </c>
       <c r="F14" s="1">
         <f t="shared" ref="F14:F30" si="3">COUNTIFS($B$49:$B$96,$A14,$D$49:$D$96,"=SIN")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" ref="G14:G30" si="4">MIN(C14,(D14/B14)*C14)</f>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="G31" s="12">
         <f>SUM(G13:G30)</f>
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>14</v>
@@ -1851,7 +1851,7 @@
         <v>25</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="E55" s="19"/>
       <c r="F55" s="20"/>

</xml_diff>